<commit_message>
Added Missing Info on Mainz
</commit_message>
<xml_diff>
--- a/Data/Hochschulkompass_Data.xlsx
+++ b/Data/Hochschulkompass_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anouk\Documents\BT\Bachelorarbeit\BA_WS25\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE37FF51-AC61-4CD0-99B5-D5AA15CD7FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9A4814-6CDE-4BD8-9A94-422776589C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2944" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2946" uniqueCount="777">
   <si>
     <t>Allgemeine Informatik</t>
   </si>
@@ -1832,12 +1832,6 @@
     <t>Imperativ, Objektorientiert</t>
   </si>
   <si>
-    <t>https://www.hs-mainz.de/studium/studiengaenge/hochschulweite-studiengaenge/angewandte-informatik-bsc/uebersicht/</t>
-  </si>
-  <si>
-    <t>Modulhandbuch Download ist 404</t>
-  </si>
-  <si>
     <t>https://www.cb.hs-mittweida.de/studienangebote-der-fakultaet/angewandte-informatik-bachelor/
 https://moodle.hs-mittweida.de/pluginfile.php/1140/coursecat/description/Modulhandbuch-Bachelor-aIF.pdf</t>
   </si>
@@ -2459,6 +2453,13 @@
   </si>
   <si>
     <t>https://code.berlin/content/uploads/1c21de3b.pdf</t>
+  </si>
+  <si>
+    <t>https://www.hs-mainz.de/studium/studiengaenge/hochschulweite-studiengaenge/angewandte-informatik-bsc/uebersicht/
+https://www.hs-mainz.de/fileadmin/Wirtschaft/Studiengaenge/bachelor/angewandte_informatik_bsc/pdf/Modulhandbuch_AI_BSc.pdf</t>
+  </si>
+  <si>
+    <t>C wird zur Einführung in die Programmierung verwendet, es scheint allerdings im weiteren Verlauf des Kurses ein Fokus auf Objektorientierter Programmierung zu sein</t>
   </si>
 </sst>
 </file>
@@ -2549,7 +2550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2572,7 +2573,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2878,8 +2882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103:XFD103"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3316,32 +3320,36 @@
         <v>597</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="10" t="s">
+      <c r="C15" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>598</v>
-      </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10" t="s">
-        <v>599</v>
+      <c r="F15" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>775</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>618</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>691</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>776</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3364,7 +3372,7 @@
         <v>5</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="H16" t="s">
         <v>584</v>
@@ -3393,7 +3401,7 @@
         <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="H17" t="s">
         <v>594</v>
@@ -3402,7 +3410,7 @@
         <v>574</v>
       </c>
       <c r="J17" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3424,8 +3432,8 @@
       <c r="F18" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="14" t="s">
-        <v>603</v>
+      <c r="G18" t="s">
+        <v>601</v>
       </c>
       <c r="H18" t="s">
         <v>584</v>
@@ -3454,7 +3462,7 @@
         <v>5</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="H19" t="s">
         <v>584</v>
@@ -3483,7 +3491,7 @@
         <v>5</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="H20" t="s">
         <v>584</v>
@@ -3512,7 +3520,7 @@
         <v>5</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="H21" t="s">
         <v>576</v>
@@ -3541,7 +3549,7 @@
         <v>5</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="H22" t="s">
         <v>584</v>
@@ -3550,7 +3558,7 @@
         <v>568</v>
       </c>
       <c r="J22" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3573,10 +3581,10 @@
         <v>5</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="H23" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="I23" t="s">
         <v>568</v>
@@ -3602,12 +3610,12 @@
         <v>5</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="10" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -3630,12 +3638,12 @@
         <v>5</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="10" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3658,16 +3666,16 @@
         <v>5</v>
       </c>
       <c r="G26" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>618</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>617</v>
-      </c>
       <c r="J26" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3690,17 +3698,17 @@
         <v>5</v>
       </c>
       <c r="G27" s="11" t="s">
+        <v>617</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>619</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>621</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3723,7 +3731,7 @@
         <v>5</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="H28" t="s">
         <v>584</v>
@@ -3752,16 +3760,16 @@
         <v>5</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="H29" t="s">
+        <v>622</v>
+      </c>
+      <c r="I29" t="s">
+        <v>623</v>
+      </c>
+      <c r="J29" t="s">
         <v>624</v>
-      </c>
-      <c r="I29" t="s">
-        <v>625</v>
-      </c>
-      <c r="J29" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3784,13 +3792,13 @@
         <v>5</v>
       </c>
       <c r="G30" s="11" t="s">
+        <v>626</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>628</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>629</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>630</v>
       </c>
       <c r="J30" s="1"/>
     </row>
@@ -3814,12 +3822,12 @@
         <v>5</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="10" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3842,7 +3850,7 @@
         <v>5</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="H32" t="s">
         <v>584</v>
@@ -3851,7 +3859,7 @@
         <v>597</v>
       </c>
       <c r="J32" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -3874,13 +3882,13 @@
         <v>5</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="J33" s="1"/>
     </row>
@@ -3904,7 +3912,7 @@
         <v>5</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="H34" t="s">
         <v>584</v>
@@ -3933,10 +3941,10 @@
         <v>5</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="H35" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="I35" t="s">
         <v>597</v>
@@ -3962,16 +3970,16 @@
         <v>5</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="H36" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="I36" t="s">
         <v>568</v>
       </c>
       <c r="K36" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3994,7 +4002,7 @@
         <v>5</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="H37" t="s">
         <v>584</v>
@@ -4023,7 +4031,7 @@
         <v>5</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="H38" t="s">
         <v>584</v>
@@ -4052,16 +4060,16 @@
         <v>5</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>584</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4084,7 +4092,7 @@
         <v>5</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="H40" t="s">
         <v>576</v>
@@ -4093,7 +4101,7 @@
         <v>568</v>
       </c>
       <c r="J40" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4116,13 +4124,13 @@
         <v>5</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="H41" s="12" t="s">
+        <v>648</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>650</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>652</v>
       </c>
       <c r="J41" s="1"/>
     </row>
@@ -4146,13 +4154,13 @@
         <v>5</v>
       </c>
       <c r="G42" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="H42" t="s">
         <v>584</v>
       </c>
       <c r="I42" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4175,7 +4183,7 @@
         <v>5</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="H43" t="s">
         <v>594</v>
@@ -4204,10 +4212,10 @@
         <v>5</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="H44" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="I44" t="s">
         <v>568</v>
@@ -4233,13 +4241,13 @@
         <v>5</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>576</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="J45" s="1"/>
     </row>
@@ -4263,12 +4271,12 @@
         <v>5</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
       <c r="J46" s="10" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4291,7 +4299,7 @@
         <v>5</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="H47" t="s">
         <v>584</v>
@@ -4300,7 +4308,7 @@
         <v>568</v>
       </c>
       <c r="J47" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4323,13 +4331,13 @@
         <v>5</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="H48" t="s">
         <v>594</v>
       </c>
       <c r="I48" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4352,7 +4360,7 @@
         <v>5</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="H49" t="s">
         <v>584</v>
@@ -4381,7 +4389,7 @@
         <v>5</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="H50" t="s">
         <v>584</v>
@@ -4410,7 +4418,7 @@
         <v>5</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="H51" t="s">
         <v>584</v>
@@ -4439,7 +4447,7 @@
         <v>5</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="H52" t="s">
         <v>594</v>
@@ -4448,7 +4456,7 @@
         <v>568</v>
       </c>
       <c r="J52" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4471,7 +4479,7 @@
         <v>5</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="H53" t="s">
         <v>576</v>
@@ -4500,13 +4508,13 @@
         <v>5</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>576</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="J54" s="1"/>
     </row>
@@ -4530,7 +4538,7 @@
         <v>5</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="H55" t="s">
         <v>584</v>
@@ -4559,13 +4567,13 @@
         <v>5</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H56" t="s">
         <v>584</v>
       </c>
       <c r="I56" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4588,7 +4596,7 @@
         <v>5</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H57" t="s">
         <v>584</v>
@@ -4617,13 +4625,13 @@
         <v>5</v>
       </c>
       <c r="G58" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="H58" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="I58" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4646,13 +4654,13 @@
         <v>5</v>
       </c>
       <c r="G59" s="9" t="s">
+        <v>674</v>
+      </c>
+      <c r="H59" t="s">
+        <v>675</v>
+      </c>
+      <c r="I59" t="s">
         <v>676</v>
-      </c>
-      <c r="H59" t="s">
-        <v>677</v>
-      </c>
-      <c r="I59" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4675,7 +4683,7 @@
         <v>5</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="H60" t="s">
         <v>576</v>
@@ -4704,11 +4712,11 @@
         <v>5</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="J61" s="10"/>
     </row>
@@ -4732,7 +4740,7 @@
         <v>5</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="H62" t="s">
         <v>576</v>
@@ -4761,7 +4769,7 @@
         <v>5</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="H63" t="s">
         <v>594</v>
@@ -4770,7 +4778,7 @@
         <v>574</v>
       </c>
       <c r="J63" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4793,7 +4801,7 @@
         <v>5</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="H64" t="s">
         <v>584</v>
@@ -4822,7 +4830,7 @@
         <v>5</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="H65" t="s">
         <v>584</v>
@@ -4851,13 +4859,13 @@
         <v>5</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="H66" t="s">
         <v>594</v>
       </c>
       <c r="I66" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4880,7 +4888,7 @@
         <v>5</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="H67" t="s">
         <v>594</v>
@@ -4889,7 +4897,7 @@
         <v>574</v>
       </c>
       <c r="J67" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4912,13 +4920,13 @@
         <v>5</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>576</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="J68" s="1"/>
     </row>
@@ -4942,13 +4950,13 @@
         <v>5</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="H69" t="s">
         <v>584</v>
       </c>
       <c r="I69" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4971,7 +4979,7 @@
         <v>5</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H70" t="s">
         <v>584</v>
@@ -5000,13 +5008,13 @@
         <v>5</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="H71" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="I71" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -5029,13 +5037,13 @@
         <v>5</v>
       </c>
       <c r="G72" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="H72" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="I72" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -5061,7 +5069,7 @@
       <c r="H73" s="10"/>
       <c r="I73" s="10"/>
       <c r="J73" s="10" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5084,7 +5092,7 @@
         <v>5</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>576</v>
@@ -5093,7 +5101,7 @@
         <v>568</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -5116,12 +5124,12 @@
         <v>5</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="H75" s="10"/>
       <c r="I75" s="10"/>
       <c r="J75" s="10" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5144,7 +5152,7 @@
         <v>5</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="H76" t="s">
         <v>576</v>
@@ -5153,7 +5161,7 @@
         <v>576</v>
       </c>
       <c r="J76" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -5176,13 +5184,13 @@
         <v>5</v>
       </c>
       <c r="G77" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="H77" t="s">
         <v>584</v>
       </c>
       <c r="I77" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5205,7 +5213,7 @@
         <v>5</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="H78" t="s">
         <v>594</v>
@@ -5234,13 +5242,13 @@
         <v>5</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="J79" s="1"/>
     </row>
@@ -5264,13 +5272,13 @@
         <v>5</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="H80" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="I80" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5293,13 +5301,13 @@
         <v>5</v>
       </c>
       <c r="G81" s="9" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="H81" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="I81" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -5322,7 +5330,7 @@
         <v>5</v>
       </c>
       <c r="G82" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="H82" t="s">
         <v>576</v>
@@ -5351,13 +5359,13 @@
         <v>5</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="H83" t="s">
         <v>584</v>
       </c>
       <c r="I83" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5380,7 +5388,7 @@
         <v>5</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="H84" t="s">
         <v>584</v>
@@ -5409,13 +5417,13 @@
         <v>5</v>
       </c>
       <c r="G85" s="11" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>576</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="J85" s="1"/>
     </row>
@@ -5439,7 +5447,7 @@
         <v>5</v>
       </c>
       <c r="G86" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="H86" t="s">
         <v>594</v>
@@ -5448,7 +5456,7 @@
         <v>576</v>
       </c>
       <c r="J86" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5471,16 +5479,16 @@
         <v>5</v>
       </c>
       <c r="G87" s="9" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="H87" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="I87" t="s">
         <v>568</v>
       </c>
       <c r="J87" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5503,7 +5511,7 @@
         <v>5</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="H88" t="s">
         <v>576</v>
@@ -5532,7 +5540,7 @@
         <v>5</v>
       </c>
       <c r="G89" s="9" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="H89" t="s">
         <v>584</v>
@@ -5541,7 +5549,7 @@
         <v>568</v>
       </c>
       <c r="J89" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5564,13 +5572,13 @@
         <v>5</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="J90" s="1"/>
     </row>
@@ -5594,13 +5602,13 @@
         <v>5</v>
       </c>
       <c r="G91" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H91" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="I91" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5623,7 +5631,7 @@
         <v>5</v>
       </c>
       <c r="G92" s="9" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="H92" t="s">
         <v>584</v>
@@ -5652,13 +5660,13 @@
         <v>5</v>
       </c>
       <c r="G93" s="9" t="s">
+        <v>727</v>
+      </c>
+      <c r="H93" t="s">
+        <v>728</v>
+      </c>
+      <c r="I93" t="s">
         <v>729</v>
-      </c>
-      <c r="H93" t="s">
-        <v>730</v>
-      </c>
-      <c r="I93" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5681,16 +5689,16 @@
         <v>5</v>
       </c>
       <c r="G94" s="9" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="H94" t="s">
         <v>584</v>
       </c>
       <c r="I94" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="J94" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5713,16 +5721,16 @@
         <v>5</v>
       </c>
       <c r="G95" s="9" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="H95" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="I95" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="J95" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5745,10 +5753,10 @@
         <v>5</v>
       </c>
       <c r="G96" s="9" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="H96" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="I96" t="s">
         <v>597</v>
@@ -5774,7 +5782,7 @@
         <v>5</v>
       </c>
       <c r="G97" s="9" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="H97" t="s">
         <v>584</v>
@@ -5803,7 +5811,7 @@
         <v>5</v>
       </c>
       <c r="G98" s="9" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="H98" t="s">
         <v>594</v>
@@ -5832,7 +5840,7 @@
         <v>5</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="H99" t="s">
         <v>576</v>
@@ -5861,7 +5869,7 @@
         <v>5</v>
       </c>
       <c r="G100" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="H100" t="s">
         <v>594</v>
@@ -5870,7 +5878,7 @@
         <v>574</v>
       </c>
       <c r="J100" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5893,16 +5901,16 @@
         <v>5</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="H101" t="s">
         <v>576</v>
       </c>
       <c r="I101" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="J101" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="102" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5925,13 +5933,13 @@
         <v>5</v>
       </c>
       <c r="G102" s="11" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>576</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5954,7 +5962,7 @@
         <v>5</v>
       </c>
       <c r="G103" s="9" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="H103" t="s">
         <v>584</v>
@@ -5983,10 +5991,10 @@
         <v>5</v>
       </c>
       <c r="G104" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="H104" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="I104" t="s">
         <v>568</v>
@@ -6012,10 +6020,10 @@
         <v>5</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="H105" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="I105" t="s">
         <v>576</v>
@@ -6041,7 +6049,7 @@
         <v>5</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="H106" t="s">
         <v>594</v>
@@ -6050,7 +6058,7 @@
         <v>576</v>
       </c>
       <c r="J106" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6073,16 +6081,16 @@
         <v>5</v>
       </c>
       <c r="G107" s="11" t="s">
+        <v>750</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="I107" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="H107" s="1" t="s">
+      <c r="J107" s="1" t="s">
         <v>753</v>
-      </c>
-      <c r="I107" s="1" t="s">
-        <v>754</v>
-      </c>
-      <c r="J107" s="1" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6105,13 +6113,13 @@
         <v>5</v>
       </c>
       <c r="G108" s="9" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="H108" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="I108" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="109" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6134,7 +6142,7 @@
         <v>5</v>
       </c>
       <c r="G109" s="9" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="H109" t="s">
         <v>584</v>
@@ -6163,13 +6171,13 @@
         <v>5</v>
       </c>
       <c r="G110" s="11" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>576</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="J110" s="1"/>
     </row>
@@ -6193,7 +6201,7 @@
         <v>5</v>
       </c>
       <c r="G111" s="9" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="H111" t="s">
         <v>584</v>
@@ -6222,13 +6230,13 @@
         <v>5</v>
       </c>
       <c r="G112" s="9" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="H112" t="s">
         <v>584</v>
       </c>
       <c r="I112" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6251,16 +6259,16 @@
         <v>5</v>
       </c>
       <c r="G113" s="11" t="s">
+        <v>761</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="J113" s="1" t="s">
         <v>763</v>
-      </c>
-      <c r="H113" s="1" t="s">
-        <v>764</v>
-      </c>
-      <c r="I113" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="J113" s="1" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
@@ -6283,7 +6291,7 @@
         <v>5</v>
       </c>
       <c r="G114" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="H114" t="s">
         <v>584</v>
@@ -6312,13 +6320,13 @@
         <v>5</v>
       </c>
       <c r="G115" s="9" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="H115" t="s">
         <v>576</v>
       </c>
       <c r="I115" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="116" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6341,13 +6349,13 @@
         <v>5</v>
       </c>
       <c r="G116" s="9" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="H116" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="I116" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6370,7 +6378,7 @@
         <v>5</v>
       </c>
       <c r="G117" s="9" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="H117" t="s">
         <v>584</v>
@@ -6399,7 +6407,7 @@
         <v>5</v>
       </c>
       <c r="G118" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="H118" t="s">
         <v>584</v>
@@ -6428,7 +6436,7 @@
         <v>5</v>
       </c>
       <c r="G119" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="H119" t="s">
         <v>576</v>
@@ -6457,13 +6465,13 @@
         <v>5</v>
       </c>
       <c r="G120" s="9" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="H120" t="s">
         <v>584</v>
       </c>
       <c r="I120" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="121" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6486,7 +6494,7 @@
         <v>5</v>
       </c>
       <c r="G121" s="9" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="H121" t="s">
         <v>576</v>
@@ -6515,7 +6523,7 @@
         <v>5</v>
       </c>
       <c r="G122" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="H122" t="s">
         <v>576</v>
@@ -6528,9 +6536,6 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G122">
     <sortCondition ref="A2:A122"/>
   </sortState>
-  <hyperlinks>
-    <hyperlink ref="G18" r:id="rId1" xr:uid="{CBD20978-25E5-4606-8913-1CB33F010243}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
 </file>

</xml_diff>